<commit_message>
modify data struct doc
</commit_message>
<xml_diff>
--- a/docs/require_documents/数据结构2018-01-29.xlsx
+++ b/docs/require_documents/数据结构2018-01-29.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="222">
   <si>
     <t>电源商（power_supplier）</t>
   </si>
@@ -653,6 +653,121 @@
   </si>
   <si>
     <t>text</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>套餐（package）</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigint</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>tinyint</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>tinyint</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>expect_price</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>预期电价</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_electricity</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>下限电量</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>decimal(16,3)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>decimal(16,3)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户-套餐映射表（user_package）</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_time</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>办理日期</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>用户</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Id</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>套餐Id</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户（user）</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>套餐（package）</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -2707,7 +2822,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:G15"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3163,7 +3278,7 @@
         <v>142</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>22</v>
+        <v>210</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>10</v>
@@ -3294,10 +3409,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3712,7 +3827,7 @@
         <v>161</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>10</v>
@@ -4168,7 +4283,7 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="3" t="s">
-        <v>59</v>
+        <v>200</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="3"/>
@@ -4301,18 +4416,268 @@
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
     </row>
+    <row r="74" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+    </row>
+    <row r="76" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="3"/>
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="3"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+    </row>
+    <row r="80" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+    </row>
+    <row r="81" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+    </row>
+    <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="3"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+    </row>
+    <row r="85" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" s="3"/>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="3"/>
+      <c r="F87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="A84:G84"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A39:G39"/>
     <mergeCell ref="A44:G44"/>
     <mergeCell ref="A50:G50"/>
     <mergeCell ref="A56:G56"/>
     <mergeCell ref="A61:G61"/>
     <mergeCell ref="A67:G67"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A39:G39"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>